<commit_message>
added more tests and updated .gitignore
</commit_message>
<xml_diff>
--- a/shared/tables/output_formats.xlsx
+++ b/shared/tables/output_formats.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="format" sheetId="1" r:id="rId1"/>
@@ -427,8 +427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,8 +527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add binning, mosaic tests
</commit_message>
<xml_diff>
--- a/shared/tables/output_formats.xlsx
+++ b/shared/tables/output_formats.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
   <si>
     <t>output_format</t>
   </si>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t>dimap.dim</t>
-  </si>
-  <si>
-    <t>netcdf4_beamnc</t>
   </si>
   <si>
     <t>csv.csv</t>
@@ -428,7 +425,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,7 +455,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -466,7 +463,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -474,7 +471,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -482,7 +479,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -490,12 +487,12 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
@@ -503,18 +500,18 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -528,7 +525,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,7 +555,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -566,7 +563,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -574,7 +571,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -582,7 +579,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -590,7 +587,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -598,7 +595,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -611,10 +608,10 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
         <v>20</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -622,7 +619,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>